<commit_message>
added NCBI ID and ITIS ID numbers
</commit_message>
<xml_diff>
--- a/Final_sample_list.xlsx
+++ b/Final_sample_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5360" yWindow="1800" windowWidth="29520" windowHeight="12400" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="15300" yWindow="460" windowWidth="18360" windowHeight="12400" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Genomes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="149">
   <si>
     <t>Genomes</t>
   </si>
@@ -388,13 +388,100 @@
   </si>
   <si>
     <t>Lamnidae (shark)</t>
+  </si>
+  <si>
+    <t>Paper cited</t>
+  </si>
+  <si>
+    <t>brain (uninjured)</t>
+  </si>
+  <si>
+    <t>spinal cord (uninjured)</t>
+  </si>
+  <si>
+    <t>late larval (5-7 yrs)</t>
+  </si>
+  <si>
+    <t>SRR5312374</t>
+  </si>
+  <si>
+    <t>Illumina HiSeq 2000</t>
+  </si>
+  <si>
+    <t>SRP101364</t>
+  </si>
+  <si>
+    <t>26.7 Gbp</t>
+  </si>
+  <si>
+    <t>SRR5312385</t>
+  </si>
+  <si>
+    <t>21.2 Gbp</t>
+  </si>
+  <si>
+    <t>https://bmcgenomics.biomedcentral.com/articles/10.1186/s12864-016-3411-x</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41598-017-18757-1</t>
+  </si>
+  <si>
+    <t>SRP095493 </t>
+  </si>
+  <si>
+    <t>SRR5124582</t>
+  </si>
+  <si>
+    <t>SRR5124576</t>
+  </si>
+  <si>
+    <t>SRR5124573</t>
+  </si>
+  <si>
+    <t>4.0 Gbp</t>
+  </si>
+  <si>
+    <t>olfactory tissue</t>
+  </si>
+  <si>
+    <t>4.7 Gbp</t>
+  </si>
+  <si>
+    <t>4.9 Gbp</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC6404594/</t>
+  </si>
+  <si>
+    <t>https://royalsocietypublishing.org/doi/full/10.1098/rspb.2017.0824?url_ver=Z39.88-2003&amp;rfr_id=ori:rid:crossref.org&amp;rfr_dat=cr_pub%3dpubmed</t>
+  </si>
+  <si>
+    <t>NCBI ID</t>
+  </si>
+  <si>
+    <t>ITIS ID</t>
+  </si>
+  <si>
+    <t>SRR3213612</t>
+  </si>
+  <si>
+    <t>SRR3213614</t>
+  </si>
+  <si>
+    <t>TSN #####</t>
+  </si>
+  <si>
+    <t>NCBI:txid####</t>
+  </si>
+  <si>
+    <t>980415 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -418,12 +505,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -431,51 +512,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -491,25 +534,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -788,723 +836,802 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L75"/>
+  <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A15" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="4" width="16.5" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" customWidth="1"/>
-    <col min="7" max="7" width="38.6640625" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" customWidth="1"/>
-    <col min="11" max="11" width="7.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="3"/>
+    <col min="2" max="2" width="26.33203125" style="3" customWidth="1"/>
+    <col min="3" max="5" width="16.5" style="3" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="21.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="38.6640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="3"/>
+    <col min="11" max="11" width="17.83203125" style="3" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="13">
+        <v>7757</v>
+      </c>
+      <c r="E2" s="13">
+        <v>159722</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="12">
         <v>885534757</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>647351933</v>
       </c>
-      <c r="D4" s="6"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="7">
         <v>25005</v>
       </c>
-      <c r="D6" s="6"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="7">
         <v>184619</v>
       </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="7">
         <v>1148</v>
       </c>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="7">
         <v>73813</v>
       </c>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="7">
         <v>13108</v>
       </c>
-      <c r="D10" s="6"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="7">
         <v>14492</v>
       </c>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="7">
         <v>73813</v>
       </c>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="J14" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" t="s">
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="I18">
+      <c r="J18" s="3">
         <v>62</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="M18" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="7">
         <v>2608383542</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="1" t="s">
+      <c r="D19" s="13">
+        <v>1855</v>
+      </c>
+      <c r="E19" s="13">
+        <v>159767</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="7">
         <v>1435388083</v>
       </c>
-      <c r="D20" s="6"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="7">
         <v>10846</v>
       </c>
-      <c r="D22" s="6"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="7">
         <v>2692996</v>
       </c>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="3">
         <v>306</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="7">
         <v>341068</v>
       </c>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="7">
         <v>7991</v>
       </c>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="7">
         <v>52630</v>
       </c>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B29" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="7">
         <v>10846</v>
       </c>
-      <c r="D29" s="6"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="1" t="s">
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E31" t="s">
+      <c r="D31" s="1">
+        <v>2056977</v>
+      </c>
+      <c r="E31" s="1">
+        <v>159671</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="L31" t="s">
+      <c r="M31" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B32" s="4" t="s">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="7">
+      <c r="C32" s="12">
         <v>643662591</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="D32" s="12"/>
+      <c r="F32" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F32" s="11" t="s">
+      <c r="G32" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="H32" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H32" s="10" t="s">
+      <c r="I32" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="L32" t="s">
+      <c r="M32" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B33" s="4" t="s">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="12">
         <v>604519456</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B34" s="4" t="s">
+      <c r="D33" s="12"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B35" s="4" t="s">
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="12">
         <v>79827</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B36" s="4" t="s">
+      <c r="D35" s="12"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="12">
         <v>259996</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B37" s="4" t="s">
+      <c r="D36" s="12"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="1">
         <v>744</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B38" s="4" t="s">
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="12">
         <v>126817</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B39" s="4" t="s">
+      <c r="D38" s="12"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="12">
         <v>20125</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B40" s="4" t="s">
+      <c r="D39" s="12"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="12">
         <v>8491</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B41" s="4" t="s">
+      <c r="D40" s="12"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B42" s="4" t="s">
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C42" s="12">
         <v>79827</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="D42" s="12"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="E48" s="4" t="s">
+      <c r="D48" s="3">
+        <v>7868</v>
+      </c>
+      <c r="E48" s="1">
+        <v>564644</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F48" s="4" t="s">
+      <c r="G48" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G48" s="4" t="s">
+      <c r="H48" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="H48" s="4" t="s">
+      <c r="I48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I48" s="4" t="s">
+      <c r="J48" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="L48" t="s">
+      <c r="M48" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E49" s="1" t="s">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F49" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="L49" t="s">
+      <c r="M49" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="50" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B50" s="4" t="s">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="7">
+      <c r="C50" s="12">
         <v>974498586</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B51" s="4" t="s">
+      <c r="D50" s="12"/>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C51" s="12">
         <v>936953458</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B52" s="4" t="s">
+      <c r="D51" s="12"/>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B52" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C52" s="4">
+      <c r="C52" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B53" s="4" t="s">
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B53" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C53" s="12">
         <v>21204</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B54" s="4" t="s">
+      <c r="D53" s="12"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B54" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C54" s="7">
+      <c r="C54" s="12">
         <v>4521921</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B55" s="4" t="s">
+      <c r="D54" s="12"/>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B55" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C55" s="4">
+      <c r="C55" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B56" s="4" t="s">
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B56" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C56" s="7">
+      <c r="C56" s="12">
         <v>67421</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B57" s="4" t="s">
+      <c r="D56" s="12"/>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B57" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C57" s="7">
+      <c r="C57" s="12">
         <v>46577</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B58" s="4" t="s">
+      <c r="D57" s="12"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B58" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C58" s="7">
+      <c r="C58" s="12">
         <v>5394</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B59" s="4" t="s">
+      <c r="D58" s="12"/>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B59" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C59" s="4">
+      <c r="C59" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B60" s="4" t="s">
+      <c r="D59" s="1"/>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B60" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C60" s="7">
+      <c r="C60" s="12">
         <v>67421</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
+      <c r="D60" s="12"/>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E63" s="1" t="s">
+      <c r="F63" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F63">
+      <c r="G63" s="3">
         <v>454</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H63" t="s">
+      <c r="I63" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J63" t="s">
+      <c r="K63" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="K63" t="s">
+      <c r="L63" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="L63" t="s">
+      <c r="M63" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="B64" s="4" t="s">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B64" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C64" s="7">
+      <c r="C64" s="12">
         <v>1030662718</v>
       </c>
-      <c r="D64" s="7"/>
-      <c r="E64" s="4" t="s">
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L64" t="s">
+      <c r="M64" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B65" s="4" t="s">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B65" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C65" s="7">
+      <c r="C65" s="12">
         <v>853439107</v>
       </c>
-      <c r="D65" s="7"/>
-    </row>
-    <row r="66" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B66" s="4" t="s">
+      <c r="D65" s="12"/>
+      <c r="E65" s="12"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B66" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C66" s="4">
+      <c r="C66" s="1">
         <v>0</v>
       </c>
-      <c r="D66" s="4"/>
-    </row>
-    <row r="67" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B67" s="4" t="s">
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B67" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C67" s="7">
+      <c r="C67" s="12">
         <v>86125</v>
       </c>
-      <c r="D67" s="7"/>
-    </row>
-    <row r="68" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B68" s="4" t="s">
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B68" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C68" s="7">
+      <c r="C68" s="12">
         <v>1051965</v>
       </c>
-      <c r="D68" s="7"/>
-    </row>
-    <row r="69" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B69" s="4" t="s">
+      <c r="D68" s="12"/>
+      <c r="E68" s="12"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B69" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C69" s="4">
+      <c r="C69" s="1">
         <v>203</v>
       </c>
-      <c r="D69" s="4"/>
-    </row>
-    <row r="70" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B70" s="4" t="s">
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B70" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C70" s="7">
+      <c r="C70" s="12">
         <v>179499</v>
       </c>
-      <c r="D70" s="7"/>
-    </row>
-    <row r="71" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B71" s="4" t="s">
+      <c r="D70" s="12"/>
+      <c r="E70" s="12"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B71" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C71" s="7">
+      <c r="C71" s="12">
         <v>9240</v>
       </c>
-      <c r="D71" s="7"/>
-    </row>
-    <row r="72" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B72" s="4" t="s">
+      <c r="D71" s="12"/>
+      <c r="E71" s="12"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B72" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C72" s="7">
+      <c r="C72" s="12">
         <v>23683</v>
       </c>
-      <c r="D72" s="7"/>
-    </row>
-    <row r="73" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B73" s="4" t="s">
+      <c r="D72" s="12"/>
+      <c r="E72" s="12"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B73" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C73" s="4">
+      <c r="C73" s="1">
         <v>0</v>
       </c>
-      <c r="D73" s="4"/>
-    </row>
-    <row r="74" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="B74" s="4" t="s">
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B74" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C74" s="7">
+      <c r="C74" s="12">
         <v>179499</v>
       </c>
-      <c r="D74" s="7"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="1" t="s">
+      <c r="D74" s="12"/>
+      <c r="E74" s="12"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="5" t="s">
         <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" tooltip="Genome assembly info"/>
-    <hyperlink ref="L18" r:id="rId2"/>
-    <hyperlink ref="E18" r:id="rId3" tooltip="Genome assembly info"/>
-    <hyperlink ref="E63" r:id="rId4" tooltip="Genome assembly info"/>
+    <hyperlink ref="F2" r:id="rId1" tooltip="Genome assembly info"/>
+    <hyperlink ref="M18" r:id="rId2"/>
+    <hyperlink ref="F18" r:id="rId3" tooltip="Genome assembly info"/>
+    <hyperlink ref="F63" r:id="rId4" tooltip="Genome assembly info"/>
     <hyperlink ref="A15" r:id="rId5"/>
     <hyperlink ref="A75" r:id="rId6"/>
-    <hyperlink ref="E19" r:id="rId7"/>
+    <hyperlink ref="F19" r:id="rId7"/>
     <hyperlink ref="A31" r:id="rId8"/>
-    <hyperlink ref="E32" r:id="rId9"/>
+    <hyperlink ref="F32" r:id="rId9"/>
     <hyperlink ref="A48" r:id="rId10"/>
-    <hyperlink ref="E49" r:id="rId11"/>
+    <hyperlink ref="F49" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1512,266 +1639,577 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" customWidth="1"/>
-    <col min="6" max="6" width="44.1640625" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="25.5" customWidth="1"/>
-    <col min="9" max="9" width="10.5" customWidth="1"/>
+    <col min="1" max="1" width="17" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="4"/>
+    <col min="6" max="7" width="10.83203125" style="14"/>
+    <col min="8" max="8" width="44.1640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="16.1640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="25.5" style="4" customWidth="1"/>
+    <col min="11" max="11" width="10.5" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>143</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" s="4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="N1" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D2" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E2" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F2" s="13">
+        <v>7750</v>
+      </c>
+      <c r="G2" s="13">
+        <v>159720</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J2" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K2" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="J3" s="12">
+      <c r="L2" s="10">
         <v>0.51</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M2" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B3" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C3" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D3" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E3" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F3" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="G3" s="13">
+        <v>622287</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J3" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K3" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="J4" s="13">
+      <c r="L3" s="15">
         <v>0.50600000000000001</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M3" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C4" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D4" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E4" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F4" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="G4" s="13">
+        <v>622287</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J4" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K4" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="J5" s="15">
+      <c r="L4" s="11">
         <v>0.45300000000000001</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M4" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="N4" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" s="13">
+        <v>7757</v>
+      </c>
+      <c r="G5" s="13">
+        <v>159722</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L5" s="11">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F6" s="13">
+        <v>7757</v>
+      </c>
+      <c r="G6" s="13">
+        <v>159722</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L6" s="11">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7" s="13">
+        <v>7757</v>
+      </c>
+      <c r="G7" s="13">
+        <v>159722</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L7" s="11">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F8" s="13">
+        <v>7757</v>
+      </c>
+      <c r="G8" s="13">
+        <v>159722</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L8" s="11">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F9" s="13">
+        <v>7757</v>
+      </c>
+      <c r="G9" s="13">
+        <v>159722</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L9" s="11">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D10" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E10" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F10" s="13">
+        <v>1855</v>
+      </c>
+      <c r="G10" s="13">
+        <v>159767</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I10" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J10" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K10" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="J8" s="15">
+      <c r="L10" s="11">
         <v>0.46300000000000002</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M10" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="L11" s="11"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="C13" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="D13" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E13" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F13" s="13">
+        <v>13397</v>
+      </c>
+      <c r="G13" s="13">
+        <v>159903</v>
+      </c>
+      <c r="H13" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="G12" t="s">
+      <c r="I13" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="H12" t="s">
+      <c r="J13" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="I12" t="s">
+      <c r="K13" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="J12" s="15">
+      <c r="L13" s="11">
         <v>0.47299999999999998</v>
       </c>
-      <c r="K12" t="s">
+      <c r="M13" s="4" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="N13" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C14" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="D14" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F14" s="13">
+        <v>170826</v>
+      </c>
+      <c r="G14" s="13">
+        <v>621035</v>
+      </c>
+      <c r="H14" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="H13" t="s">
+      <c r="J14" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="I13" t="s">
+      <c r="K14" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="J13" s="15">
+      <c r="L14" s="11">
         <v>0.44700000000000001</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M14" s="4" t="s">
         <v>112</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F17" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
-    <hyperlink ref="E4" r:id="rId2"/>
-    <hyperlink ref="E5" r:id="rId3"/>
-    <hyperlink ref="D4" r:id="rId4"/>
-    <hyperlink ref="E8" r:id="rId5"/>
-    <hyperlink ref="D8" r:id="rId6"/>
-    <hyperlink ref="E13" r:id="rId7" tooltip="Link to SRA Study"/>
-    <hyperlink ref="E12" r:id="rId8"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="D3" r:id="rId4"/>
+    <hyperlink ref="E10" r:id="rId5"/>
+    <hyperlink ref="D10" r:id="rId6"/>
+    <hyperlink ref="E14" r:id="rId7" tooltip="Link to SRA Study"/>
+    <hyperlink ref="E13" r:id="rId8"/>
+    <hyperlink ref="D6" r:id="rId9"/>
+    <hyperlink ref="E6" r:id="rId10"/>
+    <hyperlink ref="E5" r:id="rId11"/>
+    <hyperlink ref="D5" r:id="rId12"/>
+    <hyperlink ref="E7" r:id="rId13" tooltip="Link to SRA Study"/>
+    <hyperlink ref="D7" r:id="rId14"/>
+    <hyperlink ref="E9" r:id="rId15" tooltip="Link to SRA Study"/>
+    <hyperlink ref="E8" r:id="rId16" tooltip="Link to SRA Study"/>
+    <hyperlink ref="D8" r:id="rId17"/>
+    <hyperlink ref="D9" r:id="rId18"/>
+    <hyperlink ref="D14" r:id="rId19"/>
+    <hyperlink ref="D13" r:id="rId20"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
somehow left out a few lamprey/hagfish sras
</commit_message>
<xml_diff>
--- a/Final_sample_list.xlsx
+++ b/Final_sample_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15300" yWindow="460" windowWidth="18360" windowHeight="12400" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="10760" yWindow="2340" windowWidth="21520" windowHeight="14080" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Genomes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="175">
   <si>
     <t>Genomes</t>
   </si>
@@ -475,13 +475,91 @@
   </si>
   <si>
     <t>980415 </t>
+  </si>
+  <si>
+    <t>on agalma database you accidentally labelled this without the .2</t>
+  </si>
+  <si>
+    <t>Mordaciidae</t>
+  </si>
+  <si>
+    <t>Mordacia mordax</t>
+  </si>
+  <si>
+    <t>SRR2146922</t>
+  </si>
+  <si>
+    <t>SRP062082 </t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0012160616308326#s0010</t>
+  </si>
+  <si>
+    <t>seems unpaired? Check</t>
+  </si>
+  <si>
+    <t>eye</t>
+  </si>
+  <si>
+    <t>Geotria australis</t>
+  </si>
+  <si>
+    <t>Geotriidae</t>
+  </si>
+  <si>
+    <t>SRR2146917</t>
+  </si>
+  <si>
+    <t>5.2 Gbp</t>
+  </si>
+  <si>
+    <t>SRR2146918</t>
+  </si>
+  <si>
+    <t>SRR2146919</t>
+  </si>
+  <si>
+    <t>7.5 Gbp</t>
+  </si>
+  <si>
+    <t>5.3 Gbp</t>
+  </si>
+  <si>
+    <t>SRR2146912</t>
+  </si>
+  <si>
+    <t>Eptatretus cirrhatus</t>
+  </si>
+  <si>
+    <t>5.7 Gbp</t>
+  </si>
+  <si>
+    <t>SRR2146913</t>
+  </si>
+  <si>
+    <t>SRR2146914</t>
+  </si>
+  <si>
+    <t>SRR2146915</t>
+  </si>
+  <si>
+    <t>SRR2146916</t>
+  </si>
+  <si>
+    <t>6.1 Gbp</t>
+  </si>
+  <si>
+    <t>6.2 Gbp</t>
+  </si>
+  <si>
+    <t>5.5 Gbp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -512,6 +590,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -534,7 +624,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -558,6 +648,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -838,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A15" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1059,7 +1152,9 @@
       <c r="F18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G18" s="5"/>
+      <c r="G18" s="5" t="s">
+        <v>149</v>
+      </c>
       <c r="H18" s="5"/>
       <c r="I18" s="3" t="s">
         <v>42</v>
@@ -1634,15 +1729,16 @@
     <hyperlink ref="F49" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1656,7 +1752,7 @@
     <col min="8" max="8" width="44.1640625" style="4" customWidth="1"/>
     <col min="9" max="9" width="16.1640625" style="4" customWidth="1"/>
     <col min="10" max="10" width="25.5" style="4" customWidth="1"/>
-    <col min="11" max="11" width="10.5" style="4" customWidth="1"/>
+    <col min="11" max="11" width="35.6640625" style="4" customWidth="1"/>
     <col min="12" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
@@ -1736,7 +1832,7 @@
         <v>89</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>87</v>
+        <v>155</v>
       </c>
       <c r="L2" s="10">
         <v>0.51</v>
@@ -2047,144 +2143,501 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="F10" s="13">
-        <v>1855</v>
-      </c>
-      <c r="G10" s="13">
-        <v>159767</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>116</v>
+        <v>150</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="F10" s="18">
+        <v>7755</v>
+      </c>
+      <c r="G10" s="19">
+        <v>159747</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>106</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>115</v>
+        <v>156</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>87</v>
       </c>
       <c r="L10" s="11">
-        <v>0.46300000000000002</v>
+        <v>0.50900000000000001</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="L11" s="11"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N10" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="F11" s="18">
+        <v>71168</v>
+      </c>
+      <c r="G11" s="19">
+        <v>159744</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L11" s="11">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="F12" s="18">
+        <v>71168</v>
+      </c>
+      <c r="G12" s="19">
+        <v>159744</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L12" s="11">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>119</v>
+        <v>158</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="F13" s="13">
-        <v>13397</v>
-      </c>
-      <c r="G13" s="13">
-        <v>159903</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>108</v>
+        <v>157</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="F13" s="18">
+        <v>71168</v>
+      </c>
+      <c r="G13" s="19">
+        <v>159744</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>109</v>
+        <v>156</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>87</v>
       </c>
       <c r="L13" s="11">
-        <v>0.47299999999999998</v>
+        <v>0.51300000000000001</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>107</v>
+        <v>163</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>118</v>
+        <v>99</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>20</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>144</v>
+        <v>21</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>101</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="F14" s="13">
-        <v>170826</v>
+        <v>1855</v>
       </c>
       <c r="G14" s="13">
-        <v>621035</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>106</v>
+        <v>159767</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>87</v>
       </c>
       <c r="L14" s="11">
+        <v>0.46300000000000002</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="F15" s="18">
+        <v>78394</v>
+      </c>
+      <c r="G15" s="19">
+        <v>159765</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L15" s="11">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="F16" s="18">
+        <v>78394</v>
+      </c>
+      <c r="G16" s="19">
+        <v>159765</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J16" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L16" s="11">
+        <v>0.47399999999999998</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="F17" s="18">
+        <v>78394</v>
+      </c>
+      <c r="G17" s="19">
+        <v>159765</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L17" s="11">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F18" s="18">
+        <v>78394</v>
+      </c>
+      <c r="G18" s="19">
+        <v>159765</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L18" s="11">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="F19" s="18">
+        <v>78394</v>
+      </c>
+      <c r="G19" s="19">
+        <v>159765</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L19" s="11">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C20" s="8"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="L20" s="11"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F22" s="13">
+        <v>13397</v>
+      </c>
+      <c r="G22" s="13">
+        <v>159903</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L22" s="11">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F23" s="13">
+        <v>170826</v>
+      </c>
+      <c r="G23" s="13">
+        <v>621035</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="L23" s="11">
         <v>0.44700000000000001</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="M23" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="N14" s="4" t="s">
+      <c r="N23" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F17" s="14" t="s">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F26" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="G17" s="14" t="s">
+      <c r="G26" s="14" t="s">
         <v>146</v>
       </c>
     </row>
@@ -2194,10 +2647,10 @@
     <hyperlink ref="E3" r:id="rId2"/>
     <hyperlink ref="E4" r:id="rId3"/>
     <hyperlink ref="D3" r:id="rId4"/>
-    <hyperlink ref="E10" r:id="rId5"/>
-    <hyperlink ref="D10" r:id="rId6"/>
-    <hyperlink ref="E14" r:id="rId7" tooltip="Link to SRA Study"/>
-    <hyperlink ref="E13" r:id="rId8"/>
+    <hyperlink ref="E14" r:id="rId5"/>
+    <hyperlink ref="D14" r:id="rId6"/>
+    <hyperlink ref="E23" r:id="rId7" tooltip="Link to SRA Study"/>
+    <hyperlink ref="E22" r:id="rId8"/>
     <hyperlink ref="D6" r:id="rId9"/>
     <hyperlink ref="E6" r:id="rId10"/>
     <hyperlink ref="E5" r:id="rId11"/>
@@ -2208,9 +2661,16 @@
     <hyperlink ref="E8" r:id="rId16" tooltip="Link to SRA Study"/>
     <hyperlink ref="D8" r:id="rId17"/>
     <hyperlink ref="D9" r:id="rId18"/>
-    <hyperlink ref="D14" r:id="rId19"/>
-    <hyperlink ref="D13" r:id="rId20"/>
+    <hyperlink ref="D23" r:id="rId19"/>
+    <hyperlink ref="D22" r:id="rId20"/>
+    <hyperlink ref="D10" r:id="rId21"/>
+    <hyperlink ref="E10" r:id="rId22" tooltip="Link to SRA Study"/>
+    <hyperlink ref="D11" r:id="rId23"/>
+    <hyperlink ref="E11:E16" r:id="rId24" tooltip="Link to SRA Study" display="SRP062082 "/>
+    <hyperlink ref="D15" r:id="rId25"/>
+    <hyperlink ref="D16:D19" r:id="rId26" display="SRR2146912"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added citation to final_sample_list
</commit_message>
<xml_diff>
--- a/Final_sample_list.xlsx
+++ b/Final_sample_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="2340" windowWidth="21520" windowHeight="14080" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="17080" yWindow="4620" windowWidth="16540" windowHeight="16500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Genomes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="177">
   <si>
     <t>Genomes</t>
   </si>
@@ -495,9 +495,6 @@
     <t>https://www.sciencedirect.com/science/article/pii/S0012160616308326#s0010</t>
   </si>
   <si>
-    <t>seems unpaired? Check</t>
-  </si>
-  <si>
     <t>eye</t>
   </si>
   <si>
@@ -553,6 +550,15 @@
   </si>
   <si>
     <t>5.5 Gbp</t>
+  </si>
+  <si>
+    <t>Petromyzontinae</t>
+  </si>
+  <si>
+    <t>listed as paired but seems unpaired</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pubmed/29610468</t>
   </si>
 </sst>
 </file>
@@ -624,7 +630,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -645,9 +651,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1737,14 +1740,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="M9" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="4" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="16.83203125" style="4" customWidth="1"/>
     <col min="3" max="3" width="25.1640625" style="4" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" style="4" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="4"/>
@@ -1832,7 +1835,7 @@
         <v>89</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="L2" s="10">
         <v>0.51</v>
@@ -1928,7 +1931,7 @@
         <v>81</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>82</v>
+        <v>174</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>1</v>
@@ -1972,7 +1975,7 @@
         <v>81</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>82</v>
+        <v>174</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>1</v>
@@ -2016,7 +2019,7 @@
         <v>81</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>82</v>
+        <v>174</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>1</v>
@@ -2060,7 +2063,7 @@
         <v>81</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>82</v>
+        <v>174</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>1</v>
@@ -2104,7 +2107,7 @@
         <v>81</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>82</v>
+        <v>174</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>1</v>
@@ -2150,23 +2153,23 @@
       <c r="C10" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="17">
         <v>7755</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="18">
         <v>159747</v>
       </c>
       <c r="H10" s="8" t="s">
         <v>106</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K10" s="4" t="s">
         <v>87</v>
@@ -2183,28 +2186,28 @@
     </row>
     <row r="11" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="E11" s="17" t="s">
+      <c r="E11" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="17">
         <v>71168</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="18">
         <v>159744</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>125</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>87</v>
@@ -2213,7 +2216,7 @@
         <v>0.52400000000000002</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N11" s="4" t="s">
         <v>154</v>
@@ -2221,28 +2224,28 @@
     </row>
     <row r="12" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="E12" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="E12" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="17">
         <v>71168</v>
       </c>
-      <c r="G12" s="19">
+      <c r="G12" s="18">
         <v>159744</v>
       </c>
       <c r="H12" s="4" t="s">
         <v>125</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>87</v>
@@ -2251,7 +2254,7 @@
         <v>0.51900000000000002</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N12" s="4" t="s">
         <v>154</v>
@@ -2259,28 +2262,28 @@
     </row>
     <row r="13" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="E13" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="E13" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="17">
         <v>71168</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="18">
         <v>159744</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>125</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>87</v>
@@ -2289,13 +2292,13 @@
         <v>0.51300000000000001</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="N13" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>99</v>
       </c>
@@ -2303,37 +2306,37 @@
         <v>20</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="F14" s="13">
-        <v>1855</v>
-      </c>
-      <c r="G14" s="13">
-        <v>159767</v>
+        <v>165</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F14" s="17">
+        <v>78394</v>
+      </c>
+      <c r="G14" s="18">
+        <v>159765</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>115</v>
+        <v>155</v>
       </c>
       <c r="K14" s="4" t="s">
         <v>87</v>
       </c>
       <c r="L14" s="11">
-        <v>0.46300000000000002</v>
+        <v>0.51600000000000001</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>103</v>
+        <v>166</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="19" x14ac:dyDescent="0.25">
@@ -2344,34 +2347,34 @@
         <v>20</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="D15" s="17" t="s">
         <v>165</v>
       </c>
-      <c r="E15" s="17" t="s">
+      <c r="D15" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="E15" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="17">
         <v>78394</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="18">
         <v>159765</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>125</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>87</v>
       </c>
       <c r="L15" s="11">
-        <v>0.51600000000000001</v>
+        <v>0.47399999999999998</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>154</v>
@@ -2385,34 +2388,34 @@
         <v>20</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="D16" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D16" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="17">
         <v>78394</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="18">
         <v>159765</v>
       </c>
       <c r="H16" s="4" t="s">
         <v>125</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K16" s="4" t="s">
         <v>87</v>
       </c>
       <c r="L16" s="11">
-        <v>0.47399999999999998</v>
+        <v>0.46700000000000003</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="N16" s="4" t="s">
         <v>154</v>
@@ -2426,25 +2429,25 @@
         <v>20</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="D17" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D17" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="17">
         <v>78394</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="18">
         <v>159765</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>125</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>87</v>
@@ -2467,31 +2470,31 @@
         <v>20</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="D18" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D18" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="17">
         <v>78394</v>
       </c>
-      <c r="G18" s="19">
+      <c r="G18" s="18">
         <v>159765</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>125</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>87</v>
       </c>
       <c r="L18" s="11">
-        <v>0.46700000000000003</v>
+        <v>0.46100000000000002</v>
       </c>
       <c r="M18" s="4" t="s">
         <v>173</v>
@@ -2500,7 +2503,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>99</v>
       </c>
@@ -2508,46 +2511,41 @@
         <v>20</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>171</v>
+        <v>21</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>101</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="F19" s="18">
-        <v>78394</v>
-      </c>
-      <c r="G19" s="19">
-        <v>159765</v>
+        <v>100</v>
+      </c>
+      <c r="F19" s="13">
+        <v>1855</v>
+      </c>
+      <c r="G19" s="13">
+        <v>159767</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>125</v>
+        <v>102</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>156</v>
+        <v>115</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>87</v>
       </c>
       <c r="L19" s="11">
-        <v>0.46100000000000002</v>
+        <v>0.46300000000000002</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="L20" s="11"/>
+        <v>176</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
@@ -2647,8 +2645,8 @@
     <hyperlink ref="E3" r:id="rId2"/>
     <hyperlink ref="E4" r:id="rId3"/>
     <hyperlink ref="D3" r:id="rId4"/>
-    <hyperlink ref="E14" r:id="rId5"/>
-    <hyperlink ref="D14" r:id="rId6"/>
+    <hyperlink ref="E19" r:id="rId5"/>
+    <hyperlink ref="D19" r:id="rId6"/>
     <hyperlink ref="E23" r:id="rId7" tooltip="Link to SRA Study"/>
     <hyperlink ref="E22" r:id="rId8"/>
     <hyperlink ref="D6" r:id="rId9"/>
@@ -2666,9 +2664,9 @@
     <hyperlink ref="D10" r:id="rId21"/>
     <hyperlink ref="E10" r:id="rId22" tooltip="Link to SRA Study"/>
     <hyperlink ref="D11" r:id="rId23"/>
-    <hyperlink ref="E11:E16" r:id="rId24" tooltip="Link to SRA Study" display="SRP062082 "/>
-    <hyperlink ref="D15" r:id="rId25"/>
-    <hyperlink ref="D16:D19" r:id="rId26" display="SRR2146912"/>
+    <hyperlink ref="E11:E15" r:id="rId24" tooltip="Link to SRA Study" display="SRP062082 "/>
+    <hyperlink ref="D14" r:id="rId25"/>
+    <hyperlink ref="D15:D18" r:id="rId26" display="SRR2146912"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
updated final sample list
</commit_message>
<xml_diff>
--- a/Final_sample_list.xlsx
+++ b/Final_sample_list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17080" yWindow="4620" windowWidth="16540" windowHeight="16500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="20140" yWindow="480" windowWidth="11540" windowHeight="15020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Genomes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="197">
   <si>
     <t>Genomes</t>
   </si>
@@ -559,13 +559,73 @@
   </si>
   <si>
     <t>https://www.ncbi.nlm.nih.gov/pubmed/29610468</t>
+  </si>
+  <si>
+    <t>Cionidae (tunicate outgroup)</t>
+  </si>
+  <si>
+    <t>Ciona robusta</t>
+  </si>
+  <si>
+    <t>SRR7851675</t>
+  </si>
+  <si>
+    <t>late tailbud</t>
+  </si>
+  <si>
+    <t>SRP161890</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pubmed/30228204</t>
+  </si>
+  <si>
+    <t>9.2 Gbp</t>
+  </si>
+  <si>
+    <t>Ciona intestinalis</t>
+  </si>
+  <si>
+    <t>SRR8111695</t>
+  </si>
+  <si>
+    <t>SRR7261739</t>
+  </si>
+  <si>
+    <t>SRP149743</t>
+  </si>
+  <si>
+    <t>late tailbud embryos</t>
+  </si>
+  <si>
+    <t>7.0 Gbp</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov//pubmed/30069052</t>
+  </si>
+  <si>
+    <t>Polycarpa mamillaris</t>
+  </si>
+  <si>
+    <t>Styelidae (tunicate outgroup)</t>
+  </si>
+  <si>
+    <t>SRR7057581</t>
+  </si>
+  <si>
+    <t>SRP142321</t>
+  </si>
+  <si>
+    <t>7.9 Gbp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transcriptome run # </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -596,18 +656,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Times"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -630,7 +678,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -652,8 +700,9 @@
     </xf>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -934,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1738,935 +1787,1078 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M9" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17" style="4" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="4"/>
-    <col min="6" max="7" width="10.83203125" style="14"/>
-    <col min="8" max="8" width="44.1640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="16.1640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="25.5" style="4" customWidth="1"/>
-    <col min="11" max="11" width="35.6640625" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="18" style="17" customWidth="1"/>
+    <col min="2" max="2" width="17" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="4"/>
+    <col min="7" max="8" width="10.83203125" style="14"/>
+    <col min="9" max="9" width="44.1640625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="25.5" style="4" customWidth="1"/>
+    <col min="12" max="12" width="29.6640625" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>142</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>143</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="13">
+      <c r="G2" s="13">
         <v>7750</v>
       </c>
-      <c r="G2" s="13">
+      <c r="H2" s="13">
         <v>159720</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="L2" s="10">
+      <c r="M2" s="10">
         <v>0.51</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="G3" s="13">
+      <c r="H3" s="13">
         <v>622287</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L3" s="15">
+      <c r="M3" s="15">
         <v>0.50600000000000001</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="N3" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B4" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="G4" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="G4" s="13">
+      <c r="H4" s="13">
         <v>622287</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L4" s="11">
+      <c r="M4" s="11">
         <v>0.45300000000000001</v>
       </c>
-      <c r="M4" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="N4" s="4" t="s">
+      <c r="O4" s="4" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="F5" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="F5" s="13">
+      <c r="G5" s="13">
         <v>7757</v>
       </c>
-      <c r="G5" s="13">
+      <c r="H5" s="13">
         <v>159722</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="I5" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L5" s="11">
+      <c r="M5" s="11">
         <v>0.51600000000000001</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="N5" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="O5" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B6" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="F6" s="13">
+      <c r="G6" s="13">
         <v>7757</v>
       </c>
-      <c r="G6" s="13">
+      <c r="H6" s="13">
         <v>159722</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="I6" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="L6" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L6" s="11">
+      <c r="M6" s="11">
         <v>0.51900000000000002</v>
       </c>
-      <c r="M6" s="4" t="s">
+      <c r="N6" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="O6" s="4" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="F7" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="F7" s="13">
+      <c r="G7" s="13">
         <v>7757</v>
       </c>
-      <c r="G7" s="13">
+      <c r="H7" s="13">
         <v>159722</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="I7" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="J7" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="K7" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="L7" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L7" s="11">
+      <c r="M7" s="11">
         <v>0.52500000000000002</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="N7" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="O7" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="17">
+        <v>53</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="F8" s="13">
+      <c r="G8" s="13">
         <v>7757</v>
       </c>
-      <c r="G8" s="13">
+      <c r="H8" s="13">
         <v>159722</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="I8" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="J8" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="K8" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="L8" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L8" s="11">
+      <c r="M8" s="11">
         <v>0.53200000000000003</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="N8" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="O8" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="F9" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="F9" s="13">
+      <c r="G9" s="13">
         <v>7757</v>
       </c>
-      <c r="G9" s="13">
+      <c r="H9" s="13">
         <v>159722</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="I9" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="J9" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="K9" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="L9" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L9" s="11">
+      <c r="M9" s="11">
         <v>0.51600000000000001</v>
       </c>
-      <c r="M9" s="4" t="s">
+      <c r="N9" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="N9" s="4" t="s">
+      <c r="O9" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="17">
+        <v>50</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="E10" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="F10" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="F10" s="17">
+      <c r="G10" s="13">
         <v>7755</v>
       </c>
-      <c r="G10" s="18">
+      <c r="H10" s="13">
         <v>159747</v>
       </c>
-      <c r="H10" s="8" t="s">
+      <c r="I10" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="K10" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="L10" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L10" s="11">
+      <c r="M10" s="11">
         <v>0.50900000000000001</v>
       </c>
-      <c r="M10" s="4" t="s">
+      <c r="N10" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="N10" s="4" t="s">
+      <c r="O10" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B11" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="E11" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="F11" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="F11" s="17">
+      <c r="G11" s="13">
         <v>71168</v>
       </c>
-      <c r="G11" s="18">
+      <c r="H11" s="13">
         <v>159744</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="K11" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="L11" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L11" s="11">
+      <c r="M11" s="11">
         <v>0.52400000000000002</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="N11" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="O11" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D12" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="E12" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="F12" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="F12" s="17">
+      <c r="G12" s="13">
         <v>71168</v>
       </c>
-      <c r="G12" s="18">
+      <c r="H12" s="13">
         <v>159744</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="I12" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="K12" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="K12" s="4" t="s">
+      <c r="L12" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L12" s="11">
+      <c r="M12" s="11">
         <v>0.51900000000000002</v>
       </c>
-      <c r="M12" s="4" t="s">
+      <c r="N12" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="N12" s="4" t="s">
+      <c r="O12" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="E13" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="F13" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="F13" s="17">
+      <c r="G13" s="13">
         <v>71168</v>
       </c>
-      <c r="G13" s="18">
+      <c r="H13" s="13">
         <v>159744</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="K13" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="K13" s="4" t="s">
+      <c r="L13" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L13" s="11">
+      <c r="M13" s="11">
         <v>0.51300000000000001</v>
       </c>
-      <c r="M13" s="4" t="s">
+      <c r="N13" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="N13" s="4" t="s">
+      <c r="O13" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B14" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="E14" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="F14" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="F14" s="17">
+      <c r="G14" s="13">
         <v>78394</v>
       </c>
-      <c r="G14" s="18">
+      <c r="H14" s="13">
         <v>159765</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="I14" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="K14" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="K14" s="4" t="s">
+      <c r="L14" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L14" s="11">
+      <c r="M14" s="11">
         <v>0.51600000000000001</v>
       </c>
-      <c r="M14" s="4" t="s">
+      <c r="N14" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="N14" s="4" t="s">
+      <c r="O14" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B15" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="D15" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="D15" s="16" t="s">
+      <c r="E15" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="F15" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="F15" s="17">
+      <c r="G15" s="13">
         <v>78394</v>
       </c>
-      <c r="G15" s="18">
+      <c r="H15" s="13">
         <v>159765</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="I15" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="K15" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="L15" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L15" s="11">
+      <c r="M15" s="11">
         <v>0.47399999999999998</v>
       </c>
-      <c r="M15" s="4" t="s">
+      <c r="N15" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="N15" s="4" t="s">
+      <c r="O15" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="D16" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="E16" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="F16" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="F16" s="17">
+      <c r="G16" s="13">
         <v>78394</v>
       </c>
-      <c r="G16" s="18">
+      <c r="H16" s="13">
         <v>159765</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="I16" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="K16" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="K16" s="4" t="s">
+      <c r="L16" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L16" s="11">
+      <c r="M16" s="11">
         <v>0.46700000000000003</v>
       </c>
-      <c r="M16" s="4" t="s">
+      <c r="N16" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="N16" s="4" t="s">
+      <c r="O16" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B17" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="D17" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="D17" s="16" t="s">
+      <c r="E17" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="F17" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="F17" s="17">
+      <c r="G17" s="13">
         <v>78394</v>
       </c>
-      <c r="G17" s="18">
+      <c r="H17" s="13">
         <v>159765</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="I17" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="K17" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="L17" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L17" s="11">
+      <c r="M17" s="11">
         <v>0.46700000000000003</v>
       </c>
-      <c r="M17" s="4" t="s">
+      <c r="N17" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="N17" s="4" t="s">
+      <c r="O17" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="17">
+        <v>54</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="C18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="D18" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="E18" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="F18" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="F18" s="17">
+      <c r="G18" s="13">
         <v>78394</v>
       </c>
-      <c r="G18" s="18">
+      <c r="H18" s="13">
         <v>159765</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="I18" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="J18" s="4" t="s">
+      <c r="K18" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="K18" s="4" t="s">
+      <c r="L18" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L18" s="11">
+      <c r="M18" s="11">
         <v>0.46100000000000002</v>
       </c>
-      <c r="M18" s="4" t="s">
+      <c r="N18" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="N18" s="4" t="s">
+      <c r="O18" s="4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="17">
+        <v>47</v>
+      </c>
+      <c r="B19" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="C19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="D19" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="E19" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="F19" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="F19" s="13">
+      <c r="G19" s="13">
         <v>1855</v>
       </c>
-      <c r="G19" s="13">
+      <c r="H19" s="13">
         <v>159767</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="I19" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="J19" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="J19" s="4" t="s">
+      <c r="K19" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="K19" s="4" t="s">
+      <c r="L19" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L19" s="11">
+      <c r="M19" s="11">
         <v>0.46300000000000002</v>
       </c>
-      <c r="M19" s="4" t="s">
+      <c r="N19" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="N19" s="4" t="s">
+      <c r="O19" s="4" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B21" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="D22" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="F22" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="F22" s="13">
+      <c r="G22" s="13">
         <v>13397</v>
       </c>
-      <c r="G22" s="13">
+      <c r="H22" s="13">
         <v>159903</v>
       </c>
-      <c r="H22" s="8" t="s">
+      <c r="I22" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="J22" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="K22" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="K22" s="4" t="s">
+      <c r="L22" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L22" s="11">
+      <c r="M22" s="11">
         <v>0.47299999999999998</v>
       </c>
-      <c r="M22" s="4" t="s">
+      <c r="N22" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="N22" s="4" t="s">
+      <c r="O22" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="17">
+        <v>55</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="D23" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="F23" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F23" s="13">
+      <c r="G23" s="13">
         <v>170826</v>
       </c>
-      <c r="G23" s="13">
+      <c r="H23" s="13">
         <v>621035</v>
       </c>
-      <c r="H23" s="8" t="s">
+      <c r="I23" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="J23" s="4" t="s">
+      <c r="K23" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="K23" s="4" t="s">
+      <c r="L23" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L23" s="11">
+      <c r="M23" s="11">
         <v>0.44700000000000001</v>
       </c>
-      <c r="M23" s="4" t="s">
+      <c r="N23" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="N23" s="4" t="s">
+      <c r="O23" s="4" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="F26" s="14" t="s">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="17">
+        <v>72</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="G24" s="13">
+        <v>2170621</v>
+      </c>
+      <c r="H24" s="13">
+        <v>159384</v>
+      </c>
+      <c r="I24" s="8"/>
+      <c r="L24" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="M24" s="11">
+        <v>0.45300000000000001</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B25" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="G25" s="14">
+        <v>7719</v>
+      </c>
+      <c r="H25" s="13">
+        <v>159113</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="M25" s="11">
+        <v>0.28699999999999998</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B26" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="G26" s="14">
+        <v>7719</v>
+      </c>
+      <c r="H26" s="13">
+        <v>159113</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="M26" s="11">
+        <v>0.311</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="D27" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="G28" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="H28" s="14" t="s">
         <v>146</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="D3" r:id="rId4"/>
-    <hyperlink ref="E19" r:id="rId5"/>
-    <hyperlink ref="D19" r:id="rId6"/>
-    <hyperlink ref="E23" r:id="rId7" tooltip="Link to SRA Study"/>
-    <hyperlink ref="E22" r:id="rId8"/>
-    <hyperlink ref="D6" r:id="rId9"/>
-    <hyperlink ref="E6" r:id="rId10"/>
-    <hyperlink ref="E5" r:id="rId11"/>
-    <hyperlink ref="D5" r:id="rId12"/>
-    <hyperlink ref="E7" r:id="rId13" tooltip="Link to SRA Study"/>
-    <hyperlink ref="D7" r:id="rId14"/>
-    <hyperlink ref="E9" r:id="rId15" tooltip="Link to SRA Study"/>
-    <hyperlink ref="E8" r:id="rId16" tooltip="Link to SRA Study"/>
-    <hyperlink ref="D8" r:id="rId17"/>
-    <hyperlink ref="D9" r:id="rId18"/>
-    <hyperlink ref="D23" r:id="rId19"/>
-    <hyperlink ref="D22" r:id="rId20"/>
-    <hyperlink ref="D10" r:id="rId21"/>
-    <hyperlink ref="E10" r:id="rId22" tooltip="Link to SRA Study"/>
-    <hyperlink ref="D11" r:id="rId23"/>
-    <hyperlink ref="E11:E15" r:id="rId24" tooltip="Link to SRA Study" display="SRP062082 "/>
-    <hyperlink ref="D14" r:id="rId25"/>
-    <hyperlink ref="D15:D18" r:id="rId26" display="SRR2146912"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="F19" r:id="rId5"/>
+    <hyperlink ref="E19" r:id="rId6"/>
+    <hyperlink ref="F23" r:id="rId7" tooltip="Link to SRA Study"/>
+    <hyperlink ref="F22" r:id="rId8"/>
+    <hyperlink ref="E6" r:id="rId9"/>
+    <hyperlink ref="F6" r:id="rId10"/>
+    <hyperlink ref="F5" r:id="rId11"/>
+    <hyperlink ref="E5" r:id="rId12"/>
+    <hyperlink ref="F7" r:id="rId13" tooltip="Link to SRA Study"/>
+    <hyperlink ref="E7" r:id="rId14"/>
+    <hyperlink ref="F9" r:id="rId15" tooltip="Link to SRA Study"/>
+    <hyperlink ref="F8" r:id="rId16" tooltip="Link to SRA Study"/>
+    <hyperlink ref="E8" r:id="rId17"/>
+    <hyperlink ref="E9" r:id="rId18"/>
+    <hyperlink ref="E23" r:id="rId19"/>
+    <hyperlink ref="E22" r:id="rId20"/>
+    <hyperlink ref="E10" r:id="rId21"/>
+    <hyperlink ref="F10" r:id="rId22" tooltip="Link to SRA Study"/>
+    <hyperlink ref="E11" r:id="rId23"/>
+    <hyperlink ref="F11:F15" r:id="rId24" tooltip="Link to SRA Study" display="SRP062082 "/>
+    <hyperlink ref="E14" r:id="rId25"/>
+    <hyperlink ref="E15:E18" r:id="rId26" display="SRR2146912"/>
+    <hyperlink ref="E25" r:id="rId27"/>
+    <hyperlink ref="F25" r:id="rId28" tooltip="Link to SRA Study"/>
+    <hyperlink ref="E27" r:id="rId29"/>
+    <hyperlink ref="E26" r:id="rId30"/>
+    <hyperlink ref="F26" r:id="rId31" tooltip="Link to SRA Study"/>
+    <hyperlink ref="E24" r:id="rId32"/>
+    <hyperlink ref="F24" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>